<commit_message>
correção de uma frase que ficou meio escrota
</commit_message>
<xml_diff>
--- a/tarefa2.xlsx
+++ b/tarefa2.xlsx
@@ -48,7 +48,7 @@
     <t xml:space="preserve">Servidor Principal</t>
   </si>
   <si>
-    <t xml:space="preserve">O cliente deseja abrir a catraca, envia essa mensagem que é concatenada com o id da catraca que quer abrir para o servidor principal</t>
+    <t xml:space="preserve">O cliente deseja abrir a catraca, essa mensagem é concatenada com o id da catraca que quer abrir e é enviada para o servidor principal</t>
   </si>
   <si>
     <t xml:space="preserve">Dispara um processo despachante que remove da mensagem o id da catraca e reenvia a mensagem para catraca escolhida</t>
@@ -57,7 +57,7 @@
     <t xml:space="preserve">rodar</t>
   </si>
   <si>
-    <t xml:space="preserve">O cliente deseja fechar a catraca, envia essa mensagem que é concatenada com o id da catraca que quer fechar para o servidor principal</t>
+    <t xml:space="preserve">O cliente deseja fechar a catraca, essa mensagem é concatenada com o id da catraca que quer fechar e é enviada para o servidor principal</t>
   </si>
   <si>
     <t xml:space="preserve">catraca Aberta</t>
@@ -208,17 +208,17 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="17.6396761133603"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="8.81781376518219"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="18.5182186234818"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="55.3441295546559"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="50.6032388663968"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="29.8866396761134"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="17.7813765182186"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="8.78542510121457"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="18.6396761133603"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="55.8097165991903"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="50.9878542510121"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="30.1012145748988"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="1" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -256,7 +256,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="41.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
mensagens adicionadas, relacionadas ao estado da catraca
</commit_message>
<xml_diff>
--- a/tarefa2.xlsx
+++ b/tarefa2.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="27">
   <si>
     <t xml:space="preserve">Mensagem</t>
   </si>
@@ -60,19 +60,34 @@
     <t xml:space="preserve">O cliente deseja fechar a catraca, essa mensagem é concatenada com o id da catraca que quer fechar e é enviada para o servidor principal</t>
   </si>
   <si>
-    <t xml:space="preserve">catraca Aberta</t>
+    <t xml:space="preserve">estado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O cliente deseja saber o estado da catraca, essa mensagem é concatenada com o id da catraca que quer saber-se a informação e é enviada para o servidor principal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">em uso</t>
   </si>
   <si>
     <t xml:space="preserve">Catraca</t>
   </si>
   <si>
+    <t xml:space="preserve">Após receber a requisição de estado, envia uma mensagem com o mesmo pro servidor principal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Direciona a mensagem para o cliente que solicitou aquela operação na catraca</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aguardando conexão</t>
+  </si>
+  <si>
+    <t xml:space="preserve">catraca aberta</t>
+  </si>
+  <si>
     <t xml:space="preserve">Após receber a requisição de abertura, se anteriormente estava fechada libera a catraca e envia a mensagem pro servidor principal</t>
   </si>
   <si>
-    <t xml:space="preserve">Direciona a mensagem para o cliente que solicitou aquela operação na catraca</t>
-  </si>
-  <si>
-    <t xml:space="preserve">catraca Fechada</t>
+    <t xml:space="preserve">catraca fechada</t>
   </si>
   <si>
     <t xml:space="preserve">Após receber a requisição de fechamento, se anteriormente estava aberta, trava a catraca e envia a mensagem pro servidor principal</t>
@@ -205,20 +220,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
+      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="17.7813765182186"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="17.8906882591093"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="18.6396761133603"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="55.8097165991903"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="50.9878542510121"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="30.1012145748988"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="18.7449392712551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="56.2388663967611"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="51.417004048583"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="30.3157894736842"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="1" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -256,7 +271,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="41.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
@@ -274,71 +289,122 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="41.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="41.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
+      <c r="B5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="E5" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="41.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
+      <c r="B7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="1" t="s">
+      <c r="E7" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="3" t="s">
-        <v>15</v>
+      <c r="B8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>